<commit_message>
JAVA 20 - NguyenThiAnhNga - Database Design 12.11.2023
</commit_message>
<xml_diff>
--- a/JAVA 20 - NguyenThiAnhNga - Database Design.xlsx
+++ b/JAVA 20 - NguyenThiAnhNga - Database Design.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E609E9-8C59-4644-B9C2-12FA650ABD5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C7CF8D-DC57-44D9-95B8-FE184260B007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1965" windowWidth="28800" windowHeight="15435" tabRatio="422" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" tabRatio="422" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B1. Mô hình quan niệm (2)" sheetId="5" r:id="rId1"/>
@@ -50,30 +50,6 @@
           </rPr>
           <t xml:space="preserve">
 thuộc tính đa trị</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Đã đặt hàng, đang đóng gói, đang giao, giao thành công, giao thất bại</t>
         </r>
       </text>
     </comment>
@@ -188,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="128">
   <si>
     <t>Xác định các đối tượng cần lưu trữ
 Xác định các thuộc tính, thông tin của từng đối tượng</t>
@@ -620,54 +596,150 @@
     <t>field 5</t>
   </si>
   <si>
-    <t>..</t>
-  </si>
-  <si>
-    <t>Field 1</t>
-  </si>
-  <si>
-    <t>Field 2</t>
-  </si>
-  <si>
-    <t>Field 3</t>
-  </si>
-  <si>
-    <t>Field 4</t>
-  </si>
-  <si>
-    <t>Field 5</t>
-  </si>
-  <si>
     <t>B2. Mô hình logic 
 ERD</t>
   </si>
   <si>
-    <t>Object 1</t>
-  </si>
-  <si>
-    <t>Att 1</t>
-  </si>
-  <si>
-    <t>Att 2</t>
-  </si>
-  <si>
-    <t>Att 3</t>
-  </si>
-  <si>
-    <t>Object 2</t>
-  </si>
-  <si>
-    <t>Object 3</t>
-  </si>
-  <si>
-    <t>Object 4</t>
+    <t>CUSTOMER</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>PHONE</t>
+  </si>
+  <si>
+    <t>ACCOUNT</t>
+  </si>
+  <si>
+    <t>ITEM</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>SIZE(s)</t>
+  </si>
+  <si>
+    <t>MATERNAL</t>
+  </si>
+  <si>
+    <t>COLOR(s)</t>
+  </si>
+  <si>
+    <t>CUSTOMER_NAME</t>
+  </si>
+  <si>
+    <t>CUSTOMER_ADDRESS</t>
+  </si>
+  <si>
+    <t>CUSTOMER_PHONE</t>
+  </si>
+  <si>
+    <t>ITEM_ID(s)</t>
+  </si>
+  <si>
+    <t>AMOUNT</t>
+  </si>
+  <si>
+    <t>ITEM_COLOR</t>
+  </si>
+  <si>
+    <t>PRICE</t>
+  </si>
+  <si>
+    <t>DELIVERR_FEE</t>
+  </si>
+  <si>
+    <t>CREATE_AT</t>
+  </si>
+  <si>
+    <t>ORDER_STATUS</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>DELIVERY_EMPLOYEE</t>
+  </si>
+  <si>
+    <t>ITEM(s)</t>
+  </si>
+  <si>
+    <t>TOTAL_OF_MONEY</t>
+  </si>
+  <si>
+    <t>EMPLOYEE</t>
+  </si>
+  <si>
+    <t>ITEM_DETAIL</t>
+  </si>
+  <si>
+    <t>ITEM_ID</t>
+  </si>
+  <si>
+    <t>SIZE</t>
+  </si>
+  <si>
+    <t>COLOR</t>
+  </si>
+  <si>
+    <t>NAME_COLOR</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>ITEM_GROUP_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ADDRESS </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KH</t>
+    </r>
+  </si>
+  <si>
+    <t>PHONE  đatrị</t>
+  </si>
+  <si>
+    <t>ITEM_GROUP KH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLOR(s) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITEM_COLOR </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -738,6 +810,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -798,7 +884,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -852,6 +938,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -865,6 +954,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -895,7 +987,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1825486</xdr:colOff>
+      <xdr:colOff>775161</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>287481</xdr:rowOff>
     </xdr:to>
@@ -1208,22 +1300,22 @@
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="23.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" style="1" customWidth="1"/>
-    <col min="8" max="11" width="22.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="30.5703125" style="1" customWidth="1"/>
-    <col min="13" max="101" width="22.7109375" style="1" customWidth="1"/>
-    <col min="102" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5546875" style="1" customWidth="1"/>
+    <col min="8" max="11" width="22.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="30.5546875" style="1" customWidth="1"/>
+    <col min="13" max="101" width="22.6640625" style="1" customWidth="1"/>
+    <col min="102" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1231,17 +1323,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+    <row r="2" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-    </row>
-    <row r="3" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+    </row>
+    <row r="3" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1249,10 +1341,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
+    <row r="4" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1260,8 +1352,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>78</v>
       </c>
@@ -1296,7 +1388,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>81</v>
       </c>
@@ -1315,7 +1407,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>82</v>
       </c>
@@ -1334,7 +1426,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>83</v>
       </c>
@@ -1351,7 +1443,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
         <v>84</v>
@@ -1366,7 +1458,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
         <v>85</v>
@@ -1381,7 +1473,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1394,7 +1486,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1407,7 +1499,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1420,7 +1512,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1433,7 +1525,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1446,7 +1538,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1459,7 +1551,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1472,7 +1564,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1485,8 +1577,8 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
@@ -1494,7 +1586,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
         <v>7</v>
       </c>
@@ -1503,48 +1595,48 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="2:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:D4"/>
@@ -1556,39 +1648,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L51"/>
+  <dimension ref="B1:O51"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D4"/>
+    <sheetView topLeftCell="A2" zoomScale="46" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="23.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" style="1" customWidth="1"/>
-    <col min="8" max="11" width="22.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="30.5703125" style="1" customWidth="1"/>
-    <col min="13" max="101" width="22.7109375" style="1" customWidth="1"/>
-    <col min="102" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5546875" style="1" customWidth="1"/>
+    <col min="8" max="14" width="22.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="30.5546875" style="1" customWidth="1"/>
+    <col min="16" max="104" width="22.6640625" style="1" customWidth="1"/>
+    <col min="105" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+    <row r="1" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-    </row>
-    <row r="3" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+    </row>
+    <row r="3" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1596,10 +1688,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
+    <row r="4" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1607,115 +1699,227 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="J9" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="C10" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="C11" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="3"/>
+        <v>97</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -1724,11 +1928,16 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1737,11 +1946,16 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1750,11 +1964,16 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -1763,8 +1982,11 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1776,8 +1998,11 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1789,8 +2014,11 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1802,8 +2030,11 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1815,9 +2046,12 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
@@ -1825,7 +2059,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
         <v>7</v>
       </c>
@@ -1834,48 +2068,48 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="2:15" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:D4"/>
@@ -1889,37 +2123,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="84" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="23.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" style="1" customWidth="1"/>
-    <col min="8" max="11" width="22.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="30.5703125" style="1" customWidth="1"/>
-    <col min="13" max="101" width="22.7109375" style="1" customWidth="1"/>
-    <col min="102" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="32.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5546875" style="1" customWidth="1"/>
+    <col min="8" max="11" width="22.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="30.5546875" style="1" customWidth="1"/>
+    <col min="13" max="101" width="22.6640625" style="1" customWidth="1"/>
+    <col min="102" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+    <row r="1" spans="2:19" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:19" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-    </row>
-    <row r="3" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+    </row>
+    <row r="3" spans="2:19" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1927,10 +2161,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
+    <row r="4" spans="2:19" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1953,7 +2187,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>36</v>
       </c>
@@ -1994,84 +2228,177 @@
       <c r="R5" s="12"/>
       <c r="S5" s="13"/>
     </row>
-    <row r="6" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+    <row r="6" spans="2:19" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+    <row r="7" spans="2:19" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+    <row r="8" spans="2:19" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="Q8" s="11"/>
     </row>
-    <row r="9" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+    <row r="9" spans="2:19" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="J9" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+    <row r="10" spans="2:19" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="Q10" s="11"/>
       <c r="R10" s="12"/>
     </row>
-    <row r="11" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+    <row r="11" spans="2:19" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -2079,10 +2406,15 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
+    <row r="12" spans="2:19" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="29" t="s">
+        <v>94</v>
+      </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -2091,10 +2423,12 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:19" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -2106,10 +2440,12 @@
       <c r="M13" s="3"/>
       <c r="Q13" s="14"/>
     </row>
-    <row r="14" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -2122,10 +2458,12 @@
       <c r="Q14" s="11"/>
       <c r="R14" s="12"/>
     </row>
-    <row r="15" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -2138,7 +2476,7 @@
       <c r="Q15" s="11"/>
       <c r="R15" s="12"/>
     </row>
-    <row r="16" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -2153,7 +2491,7 @@
       <c r="Q16" s="11"/>
       <c r="R16" s="12"/>
     </row>
-    <row r="17" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -2169,7 +2507,7 @@
       <c r="Q17" s="11"/>
       <c r="R17" s="12"/>
     </row>
-    <row r="18" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -2183,7 +2521,7 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -2197,9 +2535,9 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="25" t="s">
+    <row r="20" spans="1:18" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:18" ht="27.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="26" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="8" t="s">
@@ -2214,8 +2552,8 @@
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
     </row>
-    <row r="22" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="25"/>
+    <row r="22" spans="1:18" ht="27.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="26"/>
       <c r="B22" s="8" t="s">
         <v>23</v>
       </c>
@@ -2228,7 +2566,7 @@
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
     </row>
-    <row r="23" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="27.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="8"/>
       <c r="C23" s="8" t="s">
         <v>24</v>
@@ -2241,9 +2579,9 @@
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
     </row>
-    <row r="24" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="26" t="s">
-        <v>92</v>
+    <row r="24" spans="1:18" ht="27.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="27" t="s">
+        <v>86</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>25</v>
@@ -2257,8 +2595,8 @@
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
     </row>
-    <row r="25" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="27"/>
+    <row r="25" spans="1:18" ht="27.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="28"/>
       <c r="B25" s="9" t="s">
         <v>26</v>
       </c>
@@ -2271,7 +2609,7 @@
       </c>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" ht="27.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="8"/>
       <c r="C26" s="8" t="s">
         <v>28</v>
@@ -2282,31 +2620,31 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:18" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:18" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:18" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:18" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:18" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:18" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:D4"/>
@@ -2328,38 +2666,38 @@
       <selection activeCell="D1" sqref="D1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="23.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="30.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="36.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="53.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="28.5703125" style="1" customWidth="1"/>
-    <col min="12" max="15" width="22.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="30.5703125" style="1" customWidth="1"/>
-    <col min="17" max="105" width="22.7109375" style="1" customWidth="1"/>
-    <col min="106" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="30.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="36.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="31.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="53.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="28.5546875" style="1" customWidth="1"/>
+    <col min="12" max="15" width="22.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="30.5546875" style="1" customWidth="1"/>
+    <col min="17" max="105" width="22.6640625" style="1" customWidth="1"/>
+    <col min="106" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+    <row r="1" spans="2:23" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:23" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
+    <row r="3" spans="2:23" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="1" t="s">
@@ -2369,10 +2707,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+    <row r="4" spans="2:23" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="1" t="s">
@@ -2400,7 +2738,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:23" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="21" t="s">
         <v>36</v>
       </c>
@@ -2465,7 +2803,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:23" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
@@ -2483,7 +2821,7 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:23" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -2501,7 +2839,7 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
     </row>
-    <row r="8" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:23" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -2520,7 +2858,7 @@
       <c r="Q8" s="3"/>
       <c r="U8" s="11"/>
     </row>
-    <row r="9" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:23" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -2538,7 +2876,7 @@
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
     </row>
-    <row r="10" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:23" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -2558,7 +2896,7 @@
       <c r="U10" s="11"/>
       <c r="V10" s="12"/>
     </row>
-    <row r="11" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:23" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -2575,7 +2913,7 @@
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
     </row>
-    <row r="12" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:23" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -2593,7 +2931,7 @@
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
     </row>
-    <row r="13" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:23" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -2612,7 +2950,7 @@
       <c r="Q13" s="3"/>
       <c r="U13" s="14"/>
     </row>
-    <row r="14" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:23" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -2632,7 +2970,7 @@
       <c r="U14" s="11"/>
       <c r="V14" s="12"/>
     </row>
-    <row r="15" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:23" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -2652,7 +2990,7 @@
       <c r="U15" s="11"/>
       <c r="V15" s="12"/>
     </row>
-    <row r="16" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:23" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -2671,7 +3009,7 @@
       <c r="U16" s="11"/>
       <c r="V16" s="12"/>
     </row>
-    <row r="17" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -2691,7 +3029,7 @@
       <c r="U17" s="11"/>
       <c r="V17" s="12"/>
     </row>
-    <row r="18" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -2709,7 +3047,7 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
     </row>
-    <row r="19" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -2727,8 +3065,8 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
     </row>
-    <row r="20" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:22" ht="27.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="16"/>
       <c r="B21" s="22" t="s">
         <v>48</v>
@@ -2748,7 +3086,7 @@
       <c r="M21" s="15"/>
       <c r="N21" s="15"/>
     </row>
-    <row r="22" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:22" ht="27.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="16"/>
       <c r="B22" s="22" t="s">
         <v>49</v>
@@ -2768,7 +3106,7 @@
       <c r="M22" s="15"/>
       <c r="N22" s="15"/>
     </row>
-    <row r="23" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:22" ht="27.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="22" t="s">
         <v>50</v>
       </c>
@@ -2787,7 +3125,7 @@
       <c r="M23" s="15"/>
       <c r="N23" s="15"/>
     </row>
-    <row r="24" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:22" ht="27.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="22" t="s">
         <v>51</v>
       </c>
@@ -2804,7 +3142,7 @@
       <c r="M24" s="15"/>
       <c r="N24" s="15"/>
     </row>
-    <row r="25" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:22" ht="27.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -2817,34 +3155,34 @@
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
     </row>
-    <row r="26" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:22" ht="27.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="L26" s="8"/>
     </row>
-    <row r="27" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:22" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:22" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:22" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:22" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:22" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:22" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:D4"/>
@@ -2863,133 +3201,133 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="23.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="255.5703125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="255.5546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>